<commit_message>
Initial importer changes and test.
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Axiom_sample_preparation_v4_9_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Axiom_sample_preparation_v4_9_0.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="G6" authorId="0">
@@ -2118,7 +2118,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD996"/>
+  <dimension ref="A1:AD997"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -2390,94 +2390,83 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="12"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
@@ -2486,7 +2475,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
+      <c r="AB8" s="12"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
@@ -5306,7 +5295,7 @@
       <c r="AC96" s="2"/>
       <c r="AD96" s="2"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -5336,6 +5325,7 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
       <c r="AC97" s="2"/>
+      <c r="AD97" s="2"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2"/>
@@ -33206,6 +33196,37 @@
       <c r="AB996" s="2"/>
       <c r="AC996" s="2"/>
     </row>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A997" s="2"/>
+      <c r="B997" s="2"/>
+      <c r="C997" s="2"/>
+      <c r="D997" s="2"/>
+      <c r="E997" s="2"/>
+      <c r="F997" s="2"/>
+      <c r="G997" s="2"/>
+      <c r="H997" s="2"/>
+      <c r="I997" s="2"/>
+      <c r="J997" s="2"/>
+      <c r="K997" s="2"/>
+      <c r="L997" s="2"/>
+      <c r="M997" s="2"/>
+      <c r="N997" s="2"/>
+      <c r="O997" s="2"/>
+      <c r="P997" s="2"/>
+      <c r="Q997" s="2"/>
+      <c r="R997" s="2"/>
+      <c r="S997" s="2"/>
+      <c r="T997" s="2"/>
+      <c r="U997" s="2"/>
+      <c r="V997" s="2"/>
+      <c r="W997" s="2"/>
+      <c r="X997" s="2"/>
+      <c r="Y997" s="2"/>
+      <c r="Z997" s="2"/>
+      <c r="AA997" s="2"/>
+      <c r="AB997" s="2"/>
+      <c r="AC997" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A5:E5"/>
@@ -33214,23 +33235,23 @@
     <mergeCell ref="P5:S5"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J8:J97" type="list">
       <formula1>Index!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:R96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R8:R97" type="list">
       <formula1>Index!$H$2:$H$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I8:I97" type="list">
       <formula1>Index!$H$2:$H$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N7:N96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N8:N97" type="list">
       <formula1>Index!$H$2:$H$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E8:E97" type="list">
       <formula1>Index!$I$2:$I$4</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Tests and changes for additional templates.
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Axiom_sample_preparation_v4_9_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Axiom_sample_preparation_v4_9_0.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="G6" authorId="0">
@@ -2118,7 +2118,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD996"/>
+  <dimension ref="A1:AD997"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -2390,94 +2390,83 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="12"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
@@ -2486,7 +2475,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
+      <c r="AB8" s="12"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
@@ -5306,7 +5295,7 @@
       <c r="AC96" s="2"/>
       <c r="AD96" s="2"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -5336,6 +5325,7 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
       <c r="AC97" s="2"/>
+      <c r="AD97" s="2"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2"/>
@@ -33206,6 +33196,37 @@
       <c r="AB996" s="2"/>
       <c r="AC996" s="2"/>
     </row>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A997" s="2"/>
+      <c r="B997" s="2"/>
+      <c r="C997" s="2"/>
+      <c r="D997" s="2"/>
+      <c r="E997" s="2"/>
+      <c r="F997" s="2"/>
+      <c r="G997" s="2"/>
+      <c r="H997" s="2"/>
+      <c r="I997" s="2"/>
+      <c r="J997" s="2"/>
+      <c r="K997" s="2"/>
+      <c r="L997" s="2"/>
+      <c r="M997" s="2"/>
+      <c r="N997" s="2"/>
+      <c r="O997" s="2"/>
+      <c r="P997" s="2"/>
+      <c r="Q997" s="2"/>
+      <c r="R997" s="2"/>
+      <c r="S997" s="2"/>
+      <c r="T997" s="2"/>
+      <c r="U997" s="2"/>
+      <c r="V997" s="2"/>
+      <c r="W997" s="2"/>
+      <c r="X997" s="2"/>
+      <c r="Y997" s="2"/>
+      <c r="Z997" s="2"/>
+      <c r="AA997" s="2"/>
+      <c r="AB997" s="2"/>
+      <c r="AC997" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A5:E5"/>
@@ -33214,23 +33235,23 @@
     <mergeCell ref="P5:S5"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J8:J97" type="list">
       <formula1>Index!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:R96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R8:R97" type="list">
       <formula1>Index!$H$2:$H$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I8:I97" type="list">
       <formula1>Index!$H$2:$H$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N7:N96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N8:N97" type="list">
       <formula1>Index!$H$2:$H$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E96" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E8:E97" type="list">
       <formula1>Index!$I$2:$I$4</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>